<commit_message>
added tests for Gradebook class
</commit_message>
<xml_diff>
--- a/Labs/PDP-Lab3/examples.xlsx
+++ b/Labs/PDP-Lab3/examples.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t xml:space="preserve">Amit</t>
   </si>
@@ -64,10 +64,70 @@
     <t xml:space="preserve">Chitnis</t>
   </si>
   <si>
-    <t xml:space="preserve">Sumeet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gajjar</t>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Builder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fname10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lname10</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;-</t>
@@ -217,10 +277,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -398,32 +458,381 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <f aca="false">SUMPRODUCT(C7:F7,finalscores!A$1:D$1)</f>
         <v>100</v>
       </c>
-      <c r="I7" s="0" t="str">
+      <c r="I7" s="1" t="str">
         <f aca="false">VLOOKUP(H7,gradeboundaries,2)</f>
         <v>A</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C8:F8,finalscores!A$1:D$1)</f>
+        <v>100</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f aca="false">VLOOKUP(H8,gradeboundaries,2)</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C9:F9,finalscores!A$1:D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f aca="false">VLOOKUP(H9,gradeboundaries,2)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C10:F10,finalscores!A$1:D$1)</f>
+        <v>20</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f aca="false">VLOOKUP(H10,gradeboundaries,2)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C11:F11,finalscores!A$1:D$1)</f>
+        <v>30</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f aca="false">VLOOKUP(H11,gradeboundaries,2)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C12:F12,finalscores!A$1:D$1)</f>
+        <v>40</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f aca="false">VLOOKUP(H12,gradeboundaries,2)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C13:F13,finalscores!A$1:D$1)</f>
+        <v>10</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f aca="false">VLOOKUP(H13,gradeboundaries,2)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C14:F14,finalscores!A$1:D$1)</f>
+        <v>84</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f aca="false">VLOOKUP(H14,gradeboundaries,2)</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C15:F15,finalscores!A$1:D$1)</f>
+        <v>82</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f aca="false">VLOOKUP(H15,gradeboundaries,2)</f>
+        <v>B-</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C16:F16,finalscores!A$1:D$1)</f>
+        <v>76</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f aca="false">VLOOKUP(H16,gradeboundaries,2)</f>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C17:F17,finalscores!A$1:D$1)</f>
+        <v>82</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f aca="false">VLOOKUP(H17,gradeboundaries,2)</f>
+        <v>B-</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C18:F18,finalscores!A$1:D$1)</f>
+        <v>62.8</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f aca="false">VLOOKUP(H18,gradeboundaries,2)</f>
+        <v>D-</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="n">
+        <f aca="false">SUMPRODUCT(C19:F19,finalscores!A$1:D$1)</f>
+        <v>80.2</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f aca="false">VLOOKUP(H19,gradeboundaries,2)</f>
+        <v>B-</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -465,10 +874,10 @@
         <v>10</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,10 +886,10 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -489,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -498,7 +907,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -507,7 +916,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -516,7 +925,7 @@
         <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -525,7 +934,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -534,7 +943,7 @@
         <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -543,7 +952,7 @@
         <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -552,7 +961,7 @@
         <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -561,7 +970,7 @@
         <v>83</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -570,7 +979,7 @@
         <v>86</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -579,7 +988,7 @@
         <v>90</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -588,7 +997,7 @@
         <v>93</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,7 +1005,7 @@
         <v>100</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed test by changing the input
</commit_message>
<xml_diff>
--- a/Labs/PDP-Lab3/examples.xlsx
+++ b/Labs/PDP-Lab3/examples.xlsx
@@ -280,7 +280,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -470,14 +470,14 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="n">
         <f aca="false">SUMPRODUCT(C7:F7,finalscores!A$1:D$1)</f>
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I7" s="1" t="str">
         <f aca="false">VLOOKUP(H7,gradeboundaries,2)</f>
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>1</v>
@@ -506,7 +506,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="n">
         <f aca="false">SUMPRODUCT(C8:F8,finalscores!A$1:D$1)</f>
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I8" s="1" t="str">
         <f aca="false">VLOOKUP(H8,gradeboundaries,2)</f>

</xml_diff>

<commit_message>
bug fix for lettergrade method
</commit_message>
<xml_diff>
--- a/Labs/PDP-Lab3/examples.xlsx
+++ b/Labs/PDP-Lab3/examples.xlsx
@@ -470,14 +470,14 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="n">
         <f aca="false">SUMPRODUCT(C7:F7,finalscores!A$1:D$1)</f>
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I7" s="1" t="str">
         <f aca="false">VLOOKUP(H7,gradeboundaries,2)</f>
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>1</v>
@@ -506,7 +506,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="n">
         <f aca="false">SUMPRODUCT(C8:F8,finalscores!A$1:D$1)</f>
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I8" s="1" t="str">
         <f aca="false">VLOOKUP(H8,gradeboundaries,2)</f>

</xml_diff>